<commit_message>
agregar picker al mapa
</commit_message>
<xml_diff>
--- a/api/db/sesiones/sesion_3000.xlsx
+++ b/api/db/sesiones/sesion_3000.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alienware\Desktop\Proyectos software\EOLO_WEBAPP\api\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EE1EBF-33A5-45B4-B2CD-EE3F361C93A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F56780-75D7-4650-8F11-C2A98B99E1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>Eolo_MP_300</t>
   </si>
   <si>
-    <t>Concepcion</t>
-  </si>
-  <si>
     <t>Modelo 3.0</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>ubicacion</t>
+  </si>
+  <si>
+    <t>Santiago, Chile</t>
   </si>
 </sst>
 </file>
@@ -394,14 +394,15 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -421,19 +422,19 @@
         <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
       <c r="H1" t="s">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -456,13 +457,13 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2">
         <v>50</v>
@@ -488,13 +489,13 @@
         <v>0.83333333333333304</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3">
         <v>20</v>
@@ -520,13 +521,13 @@
         <v>0.875</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4">
         <v>30</v>
@@ -552,13 +553,13 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <v>50</v>
@@ -584,13 +585,13 @@
         <v>0.95833333333333304</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6">
         <v>10</v>
@@ -616,13 +617,13 @@
         <v>0.999999999999999</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7">
         <v>30</v>
@@ -648,13 +649,13 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8">
         <v>50</v>
@@ -680,13 +681,13 @@
         <v>8.3333333333338894E-2</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9">
         <v>20</v>
@@ -712,13 +713,13 @@
         <v>0.124999999999999</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10">
         <v>20</v>
@@ -744,13 +745,13 @@
         <v>0.16666666666666899</v>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J11">
         <v>50</v>
@@ -776,13 +777,13 @@
         <v>0.208333333333339</v>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12">
         <v>30</v>
@@ -808,13 +809,13 @@
         <v>0.25000000000000899</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13">
         <v>50</v>
@@ -840,13 +841,13 @@
         <v>0.29166666666666902</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J14">
         <v>20</v>
@@ -872,13 +873,13 @@
         <v>0.33333333333333898</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J15">
         <v>50</v>
@@ -904,13 +905,13 @@
         <v>0.37500000000000999</v>
       </c>
       <c r="G16" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J16">
         <v>30</v>
@@ -936,13 +937,13 @@
         <v>0.41666666666667901</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J17">
         <v>10</v>
@@ -968,13 +969,13 @@
         <v>0.45833333333329801</v>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J18">
         <v>30</v>
@@ -1000,13 +1001,13 @@
         <v>0.499999999999998</v>
       </c>
       <c r="G19" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J19">
         <v>50</v>
@@ -1032,13 +1033,13 @@
         <v>0.54166666666669805</v>
       </c>
       <c r="G20" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J20">
         <v>30</v>

</xml_diff>